<commit_message>
Added more details to readme. Extracted data from 2022 AWLA survey to parental leave data.xlsx.
</commit_message>
<xml_diff>
--- a/parental leave data.xlsx
+++ b/parental leave data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t xml:space="preserve">firm</t>
   </si>
@@ -29,6 +29,9 @@
     <t xml:space="preserve">year</t>
   </si>
   <si>
+    <t xml:space="preserve">response</t>
+  </si>
+  <si>
     <t xml:space="preserve">firm_type</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
     <t xml:space="preserve">AJ Park</t>
   </si>
   <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anderson Lloyd</t>
   </si>
   <si>
@@ -71,7 +77,7 @@
     <t xml:space="preserve">Davenports</t>
   </si>
   <si>
-    <t xml:space="preserve">no response</t>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">Dentons Kensington Swan</t>
@@ -107,6 +113,9 @@
     <t xml:space="preserve">Hudson Gavin Martin</t>
   </si>
   <si>
+    <t xml:space="preserve">all details noted as ‘commercially sensitive’</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lane Neave</t>
   </si>
   <si>
@@ -164,7 +173,10 @@
     <t xml:space="preserve">Name of Law Firm</t>
   </si>
   <si>
-    <t xml:space="preserve">Anna’s ranking system of firms: 1 – Large high-tier, 2 – Boutique high tier, 3 – boutique medium tier, 4 – other</t>
+    <t xml:space="preserve">reponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates if the firm responded to the survey or gave no response</t>
   </si>
   <si>
     <t xml:space="preserve">Period of paid parental leave for a primary carer (in weeks)</t>
@@ -198,10 +210,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -274,11 +285,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -471,551 +482,740 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="9.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="58.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="str">
+      <c r="G2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="str">
         <f aca="false">B2&amp;"_"&amp;SUBSTITUTE(LOWER(A2)," ","_")</f>
         <v>2022_aj_park</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H3" s="0" t="str">
+      <c r="G3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1" t="str">
         <f aca="false">B3&amp;"_"&amp;SUBSTITUTE(LOWER(A3)," ","_")</f>
         <v>2022_anderson_lloyd</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H4" s="0" t="str">
+      <c r="I4" s="1" t="str">
         <f aca="false">B4&amp;"_"&amp;SUBSTITUTE(LOWER(A4)," ","_")</f>
         <v>2022_anthony_harper</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="0" t="str">
+      <c r="I5" s="1" t="str">
         <f aca="false">B5&amp;"_"&amp;SUBSTITUTE(LOWER(A5)," ","_")</f>
         <v>2022_bell_gully</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="0" t="str">
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="str">
         <f aca="false">B6&amp;"_"&amp;SUBSTITUTE(LOWER(A6)," ","_")</f>
         <v>2022_buddle_findlay</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="H7" s="0" t="str">
+      <c r="I7" s="1" t="str">
         <f aca="false">B7&amp;"_"&amp;SUBSTITUTE(LOWER(A7)," ","_")</f>
         <v>2022_chapman_tripp</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="0" t="str">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1" t="str">
         <f aca="false">B8&amp;"_"&amp;SUBSTITUTE(LOWER(A8)," ","_")</f>
         <v>2022_davenports</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="H9" s="0" t="str">
+      <c r="E9" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="str">
         <f aca="false">B9&amp;"_"&amp;SUBSTITUTE(LOWER(A9)," ","_")</f>
         <v>2022_dentons_kensington_swan</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="0" t="str">
+      <c r="E10" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1" t="str">
         <f aca="false">B10&amp;"_"&amp;SUBSTITUTE(LOWER(A10)," ","_")</f>
         <v>2022_dla_piper</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H11" s="0" t="str">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="str">
         <f aca="false">B11&amp;"_"&amp;SUBSTITUTE(LOWER(A11)," ","_")</f>
         <v>2022_duncan_cotterill</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H12" s="0" t="str">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="1" t="str">
         <f aca="false">B12&amp;"_"&amp;SUBSTITUTE(LOWER(A12)," ","_")</f>
         <v>2022_gilbert_walker</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H13" s="0" t="str">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="1" t="str">
         <f aca="false">B13&amp;"_"&amp;SUBSTITUTE(LOWER(A13)," ","_")</f>
         <v>2022_glaistor_ennor</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H14" s="0" t="str">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="1" t="str">
         <f aca="false">B14&amp;"_"&amp;SUBSTITUTE(LOWER(A14)," ","_")</f>
         <v>2022_greenwood_roche</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H15" s="0" t="str">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="1" t="str">
         <f aca="false">B15&amp;"_"&amp;SUBSTITUTE(LOWER(A15)," ","_")</f>
         <v>2022_grimshaw_&amp;_co</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H16" s="0" t="str">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="str">
         <f aca="false">B16&amp;"_"&amp;SUBSTITUTE(LOWER(A16)," ","_")</f>
         <v>2022_haigh_lyon</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H17" s="0" t="str">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="1" t="str">
         <f aca="false">B17&amp;"_"&amp;SUBSTITUTE(LOWER(A17)," ","_")</f>
         <v>2022_harmon_horton_lusk</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H18" s="0" t="str">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="str">
         <f aca="false">B18&amp;"_"&amp;SUBSTITUTE(LOWER(A18)," ","_")</f>
         <v>2022_hesketh_henry</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H19" s="0" t="str">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="1" t="str">
         <f aca="false">B19&amp;"_"&amp;SUBSTITUTE(LOWER(A19)," ","_")</f>
         <v>2022_hudson_gavin_martin</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H20" s="0" t="str">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="1" t="str">
         <f aca="false">B20&amp;"_"&amp;SUBSTITUTE(LOWER(A20)," ","_")</f>
         <v>2022_lane_neave</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H21" s="2" t="str">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="1" t="str">
         <f aca="false">B21&amp;"_"&amp;SUBSTITUTE(LOWER(A21)," ","_")</f>
         <v>2022_lee_salmon_long</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H22" s="2" t="str">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="1" t="str">
         <f aca="false">B22&amp;"_"&amp;SUBSTITUTE(LOWER(A22)," ","_")</f>
         <v>2022_lowndes_jordan</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H23" s="2" t="str">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="1" t="str">
         <f aca="false">B23&amp;"_"&amp;SUBSTITUTE(LOWER(A23)," ","_")</f>
         <v>2022_martelli_mckegg</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H24" s="2" t="str">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="1" t="str">
         <f aca="false">B24&amp;"_"&amp;SUBSTITUTE(LOWER(A24)," ","_")</f>
         <v>2022_mayne_wetherll</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H25" s="2" t="str">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="str">
         <f aca="false">B25&amp;"_"&amp;SUBSTITUTE(LOWER(A25)," ","_")</f>
         <v>2022_mcveagh_fleming</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H26" s="2" t="str">
+      <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1" t="str">
         <f aca="false">B26&amp;"_"&amp;SUBSTITUTE(LOWER(A26)," ","_")</f>
         <v>2022_meredith_connell</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H27" s="2" t="str">
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1" t="str">
         <f aca="false">B27&amp;"_"&amp;SUBSTITUTE(LOWER(A27)," ","_")</f>
         <v>2022_minter_ellison_rudd_watts</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H28" s="2" t="str">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="1" t="str">
         <f aca="false">B28&amp;"_"&amp;SUBSTITUTE(LOWER(A28)," ","_")</f>
         <v>2022_morris_legal</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H29" s="2" t="str">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="1" t="str">
         <f aca="false">B29&amp;"_"&amp;SUBSTITUTE(LOWER(A29)," ","_")</f>
         <v>2022_rice_spier</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H30" s="2" t="str">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I30" s="1" t="str">
         <f aca="false">B30&amp;"_"&amp;SUBSTITUTE(LOWER(A30)," ","_")</f>
         <v>2022_russell_mcveagh</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H31" s="2" t="str">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1" t="str">
         <f aca="false">B31&amp;"_"&amp;SUBSTITUTE(LOWER(A31)," ","_")</f>
         <v>2022_simpson_grierson</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H32" s="2" t="str">
+      <c r="A32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="1" t="str">
         <f aca="false">B32&amp;"_"&amp;SUBSTITUTE(LOWER(A32)," ","_")</f>
         <v>2022_tompkins_wake</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H33" s="2" t="str">
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1" t="str">
         <f aca="false">B33&amp;"_"&amp;SUBSTITUTE(LOWER(A33)," ","_")</f>
         <v>2022_turner_hopkins</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H34" s="2" t="str">
+      <c r="A34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="1" t="str">
         <f aca="false">B34&amp;"_"&amp;SUBSTITUTE(LOWER(A34)," ","_")</f>
         <v>2022_wilson_harle</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="H35" s="2" t="str">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="1" t="str">
         <f aca="false">B35&amp;"_"&amp;SUBSTITUTE(LOWER(A35)," ","_")</f>
         <v>2022_wynn_williams</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C36" s="0" t="n">
+      <c r="A36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="F36" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="H36" s="2" t="str">
+      <c r="I36" s="1" t="str">
         <f aca="false">B36&amp;"_"&amp;SUBSTITUTE(LOWER(A36)," ","_")</f>
         <v>2022_kindrik_partners</v>
       </c>
@@ -1036,99 +1236,111 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="73.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="73.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>47</v>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>48</v>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>49</v>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>50</v>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>55</v>
+      <c r="A15" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>56</v>
+      <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test column for firm_type.
</commit_message>
<xml_diff>
--- a/parental leave data.xlsx
+++ b/parental leave data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="65">
   <si>
     <t xml:space="preserve">firm</t>
   </si>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">firm_type</t>
   </si>
   <si>
+    <t xml:space="preserve">firm_type_ts</t>
+  </si>
+  <si>
     <t xml:space="preserve">primary_paid</t>
   </si>
   <si>
@@ -56,13 +59,22 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
+    <t xml:space="preserve">mid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anderson Lloyd</t>
   </si>
   <si>
     <t xml:space="preserve">Anthony Harper</t>
   </si>
   <si>
+    <t xml:space="preserve">low</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bell Gully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high</t>
   </si>
   <si>
     <t xml:space="preserve">Buddle Findlay</t>
@@ -482,10 +494,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -493,9 +505,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="9.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="58.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="58.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,696 +538,804 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>12</v>
-      </c>
       <c r="G2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="1" t="str">
+      <c r="J2" s="1" t="str">
         <f aca="false">B2&amp;"_"&amp;SUBSTITUTE(LOWER(A2)," ","_")</f>
         <v>2022_aj_park</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>12</v>
-      </c>
       <c r="G3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="1" t="str">
+      <c r="J3" s="1" t="str">
         <f aca="false">B3&amp;"_"&amp;SUBSTITUTE(LOWER(A3)," ","_")</f>
         <v>2022_anderson_lloyd</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="G4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="H4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="1" t="str">
+      <c r="J4" s="1" t="str">
         <f aca="false">B4&amp;"_"&amp;SUBSTITUTE(LOWER(A4)," ","_")</f>
         <v>2022_anthony_harper</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="G5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="1" t="str">
+      <c r="J5" s="1" t="str">
         <f aca="false">B5&amp;"_"&amp;SUBSTITUTE(LOWER(A5)," ","_")</f>
         <v>2022_bell_gully</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>12</v>
-      </c>
       <c r="G6" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="1" t="str">
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="1" t="str">
         <f aca="false">B6&amp;"_"&amp;SUBSTITUTE(LOWER(A6)," ","_")</f>
         <v>2022_buddle_findlay</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="I7" s="1" t="str">
+      <c r="J7" s="1" t="str">
         <f aca="false">B7&amp;"_"&amp;SUBSTITUTE(LOWER(A7)," ","_")</f>
         <v>2022_chapman_tripp</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="1" t="str">
         <f aca="false">B8&amp;"_"&amp;SUBSTITUTE(LOWER(A8)," ","_")</f>
         <v>2022_davenports</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="G9" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="H9" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I9" s="1" t="str">
+      <c r="J9" s="1" t="str">
         <f aca="false">B9&amp;"_"&amp;SUBSTITUTE(LOWER(A9)," ","_")</f>
         <v>2022_dentons_kensington_swan</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="G10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="H10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I10" s="1" t="str">
+      <c r="J10" s="1" t="str">
         <f aca="false">B10&amp;"_"&amp;SUBSTITUTE(LOWER(A10)," ","_")</f>
         <v>2022_dla_piper</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="1" t="str">
+      <c r="J11" s="1" t="str">
         <f aca="false">B11&amp;"_"&amp;SUBSTITUTE(LOWER(A11)," ","_")</f>
         <v>2022_duncan_cotterill</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1" t="str">
         <f aca="false">B12&amp;"_"&amp;SUBSTITUTE(LOWER(A12)," ","_")</f>
         <v>2022_gilbert_walker</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="1" t="str">
         <f aca="false">B13&amp;"_"&amp;SUBSTITUTE(LOWER(A13)," ","_")</f>
         <v>2022_glaistor_ennor</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="1" t="str">
         <f aca="false">B14&amp;"_"&amp;SUBSTITUTE(LOWER(A14)," ","_")</f>
         <v>2022_greenwood_roche</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1" t="str">
         <f aca="false">B15&amp;"_"&amp;SUBSTITUTE(LOWER(A15)," ","_")</f>
         <v>2022_grimshaw_&amp;_co</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="1" t="str">
+      <c r="J16" s="1" t="str">
         <f aca="false">B16&amp;"_"&amp;SUBSTITUTE(LOWER(A16)," ","_")</f>
         <v>2022_haigh_lyon</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1" t="str">
         <f aca="false">B17&amp;"_"&amp;SUBSTITUTE(LOWER(A17)," ","_")</f>
         <v>2022_harmon_horton_lusk</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="G18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="H18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="1" t="str">
+      <c r="J18" s="1" t="str">
         <f aca="false">B18&amp;"_"&amp;SUBSTITUTE(LOWER(A18)," ","_")</f>
         <v>2022_hesketh_henry</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="1" t="str">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" s="1" t="str">
         <f aca="false">B19&amp;"_"&amp;SUBSTITUTE(LOWER(A19)," ","_")</f>
         <v>2022_hudson_gavin_martin</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1" t="str">
         <f aca="false">B20&amp;"_"&amp;SUBSTITUTE(LOWER(A20)," ","_")</f>
         <v>2022_lane_neave</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="1" t="str">
         <f aca="false">B21&amp;"_"&amp;SUBSTITUTE(LOWER(A21)," ","_")</f>
         <v>2022_lee_salmon_long</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="1" t="str">
         <f aca="false">B22&amp;"_"&amp;SUBSTITUTE(LOWER(A22)," ","_")</f>
         <v>2022_lowndes_jordan</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="1" t="str">
         <f aca="false">B23&amp;"_"&amp;SUBSTITUTE(LOWER(A23)," ","_")</f>
         <v>2022_martelli_mckegg</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1" t="str">
         <f aca="false">B24&amp;"_"&amp;SUBSTITUTE(LOWER(A24)," ","_")</f>
         <v>2022_mayne_wetherll</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="1" t="n">
+      <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="1" t="str">
+      <c r="J25" s="1" t="str">
         <f aca="false">B25&amp;"_"&amp;SUBSTITUTE(LOWER(A25)," ","_")</f>
         <v>2022_mcveagh_fleming</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="G26" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="H26" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I26" s="1" t="str">
+      <c r="J26" s="1" t="str">
         <f aca="false">B26&amp;"_"&amp;SUBSTITUTE(LOWER(A26)," ","_")</f>
         <v>2022_meredith_connell</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="F27" s="1" t="n">
-        <v>12</v>
-      </c>
       <c r="G27" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I27" s="1" t="str">
+      <c r="J27" s="1" t="str">
         <f aca="false">B27&amp;"_"&amp;SUBSTITUTE(LOWER(A27)," ","_")</f>
         <v>2022_minter_ellison_rudd_watts</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="1" t="str">
         <f aca="false">B28&amp;"_"&amp;SUBSTITUTE(LOWER(A28)," ","_")</f>
         <v>2022_morris_legal</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="1" t="str">
         <f aca="false">B29&amp;"_"&amp;SUBSTITUTE(LOWER(A29)," ","_")</f>
         <v>2022_rice_spier</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="F30" s="1" t="n">
+      <c r="G30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="H30" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I30" s="1" t="str">
+      <c r="J30" s="1" t="str">
         <f aca="false">B30&amp;"_"&amp;SUBSTITUTE(LOWER(A30)," ","_")</f>
         <v>2022_russell_mcveagh</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="F31" s="1" t="n">
-        <v>12</v>
-      </c>
       <c r="G31" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I31" s="1" t="str">
+      <c r="J31" s="1" t="str">
         <f aca="false">B31&amp;"_"&amp;SUBSTITUTE(LOWER(A31)," ","_")</f>
         <v>2022_simpson_grierson</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="1" t="str">
         <f aca="false">B32&amp;"_"&amp;SUBSTITUTE(LOWER(A32)," ","_")</f>
         <v>2022_tompkins_wake</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="1" t="str">
         <f aca="false">B33&amp;"_"&amp;SUBSTITUTE(LOWER(A33)," ","_")</f>
         <v>2022_turner_hopkins</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="1" t="str">
         <f aca="false">B34&amp;"_"&amp;SUBSTITUTE(LOWER(A34)," ","_")</f>
         <v>2022_wilson_harle</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="1" t="str">
         <f aca="false">B35&amp;"_"&amp;SUBSTITUTE(LOWER(A35)," ","_")</f>
         <v>2022_wynn_williams</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>2022</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E36" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="F36" s="1" t="n">
+      <c r="G36" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="I36" s="1" t="str">
+      <c r="J36" s="1" t="str">
         <f aca="false">B36&amp;"_"&amp;SUBSTITUTE(LOWER(A36)," ","_")</f>
         <v>2022_kindrik_partners</v>
       </c>
@@ -1249,7 +1369,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1258,15 +1378,15 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,34 +1399,34 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,15 +1434,15 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1330,17 +1450,17 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the graph to make single stripchart with median annotation.
</commit_message>
<xml_diff>
--- a/parental leave data.xlsx
+++ b/parental leave data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
   <si>
     <t xml:space="preserve">firm</t>
   </si>
@@ -497,7 +497,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -971,9 +971,6 @@
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>34</v>

</xml_diff>